<commit_message>
Update of the project planning
</commit_message>
<xml_diff>
--- a/documents/ProjectPlanning.xlsx
+++ b/documents/ProjectPlanning.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Phase 6: INITIATION</t>
   </si>
   <si>
-    <t xml:space="preserve">Confirmation du cahier de charge</t>
+    <t xml:space="preserve">Redaction du cahier de charge</t>
   </si>
   <si>
     <t xml:space="preserve">YARA Mendi, KONDO-KAKOU Renauld, AGBAKU Kofi Edem</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Définition des stratégies de déploiement</t>
   </si>
   <si>
-    <t xml:space="preserve">Definition du programme et calendrier pour les livrables</t>
+    <t xml:space="preserve">Définition du programme et calendrier pour les livrables</t>
   </si>
   <si>
     <t xml:space="preserve">ADABOUNOU Vincent, YARA Mendi, KONDO-KAKOU Renauld, AGBAKU Kofi Edem</t>
@@ -431,6 +431,12 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <color rgb="FFC9211E"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
@@ -443,12 +449,6 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -474,7 +474,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,7 +526,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
     <fill>
@@ -545,6 +545,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF4F6228"/>
         <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -898,11 +904,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="11" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="16" fillId="11" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="17" fillId="11" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -914,19 +924,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -934,18 +944,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="167" fontId="11" fillId="11" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="11" fillId="12" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="11" fillId="11" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -970,10 +976,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="11" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -986,11 +988,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="11" fillId="13" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="14" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="13" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="14" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -998,7 +1008,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="13" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="14" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1006,11 +1016,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="13" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="14" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="13" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="14" borderId="9" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1018,10 +1028,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="10" borderId="17" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="10" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1050,11 +1056,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1090,7 +1096,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="14" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="15" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1098,7 +1104,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1300,7 +1306,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFE16173"/>
@@ -1348,15 +1354,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>868320</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:colOff>843120</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1086840</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:colOff>1011240</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>235440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1365,8 +1371,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="868320" y="14684040"/>
-          <a:ext cx="218520" cy="191160"/>
+          <a:off x="843120" y="14987520"/>
+          <a:ext cx="168120" cy="229320"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -1395,15 +1401,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>425880</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:colOff>363960</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>159120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>644400</xdr:colOff>
+      <xdr:colOff>531000</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>12240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1412,12 +1418,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="425880" y="14954040"/>
-          <a:ext cx="218520" cy="122760"/>
+          <a:off x="363960" y="14781240"/>
+          <a:ext cx="167040" cy="212400"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
-            <a:gd name="adj" fmla="val 50000"/>
+            <a:gd name="adj" fmla="val 48690"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -1448,9 +1454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>272520</xdr:colOff>
+      <xdr:colOff>272160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>383040</xdr:rowOff>
+      <xdr:rowOff>382680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1459,8 +1465,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10355040" y="5843880"/>
-          <a:ext cx="217080" cy="169560"/>
+          <a:off x="10352520" y="5843880"/>
+          <a:ext cx="216720" cy="169200"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -1495,9 +1501,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>271800</xdr:colOff>
+      <xdr:colOff>271440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>202320</xdr:rowOff>
+      <xdr:rowOff>201960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1507,7 +1513,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9035640" y="3873240"/>
-          <a:ext cx="217440" cy="168840"/>
+          <a:ext cx="217080" cy="168480"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -1542,9 +1548,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
+      <xdr:colOff>248760</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>248040</xdr:rowOff>
+      <xdr:rowOff>247680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1553,8 +1559,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10331640" y="5261400"/>
-          <a:ext cx="217080" cy="169200"/>
+          <a:off x="10329120" y="5261400"/>
+          <a:ext cx="216720" cy="168840"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -1583,15 +1589,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>53640</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>50760</xdr:rowOff>
+      <xdr:colOff>58680</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>270720</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>220320</xdr:rowOff>
+      <xdr:colOff>275400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>292680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1600,8 +1606,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9034920" y="4824000"/>
-          <a:ext cx="217080" cy="169560"/>
+          <a:off x="9039960" y="4334760"/>
+          <a:ext cx="216720" cy="169200"/>
         </a:xfrm>
         <a:prstGeom prst="triangle">
           <a:avLst>
@@ -1610,100 +1616,6 @@
         </a:prstGeom>
         <a:solidFill>
           <a:srgbClr val="008000"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>58680</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>275760</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>293040</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9039960" y="4334760"/>
-          <a:ext cx="217080" cy="169560"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="008000"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>41400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>202680</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>372240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10341000" y="6499800"/>
-          <a:ext cx="217080" cy="169560"/>
-        </a:xfrm>
-        <a:prstGeom prst="triangle">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffff00"/>
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
@@ -1753,7 +1665,7 @@
   </sheetPr>
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -2046,10 +1958,10 @@
   </sheetPr>
   <dimension ref="A1:BH52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="6" topLeftCell="D40" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="6" topLeftCell="D20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2956,60 +2868,60 @@
       <c r="B16" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="37"/>
-      <c r="O16" s="33"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="28"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="28"/>
-      <c r="S16" s="34"/>
-      <c r="T16" s="33"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="34"/>
       <c r="U16" s="28"/>
       <c r="V16" s="28"/>
       <c r="W16" s="28"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="33"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="34"/>
       <c r="Z16" s="28"/>
       <c r="AA16" s="28"/>
       <c r="AB16" s="28"/>
-      <c r="AC16" s="34"/>
-      <c r="AD16" s="33"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="34"/>
       <c r="AE16" s="28"/>
       <c r="AF16" s="28"/>
       <c r="AG16" s="28"/>
-      <c r="AH16" s="34"/>
-      <c r="AI16" s="33"/>
+      <c r="AH16" s="35"/>
+      <c r="AI16" s="34"/>
       <c r="AJ16" s="28"/>
       <c r="AK16" s="28"/>
       <c r="AL16" s="28"/>
-      <c r="AM16" s="34"/>
-      <c r="AN16" s="33"/>
+      <c r="AM16" s="35"/>
+      <c r="AN16" s="34"/>
       <c r="AO16" s="28"/>
       <c r="AP16" s="28"/>
       <c r="AQ16" s="28"/>
-      <c r="AR16" s="34"/>
-      <c r="AS16" s="33"/>
+      <c r="AR16" s="35"/>
+      <c r="AS16" s="34"/>
       <c r="AT16" s="28"/>
       <c r="AU16" s="28"/>
       <c r="AV16" s="28"/>
-      <c r="AW16" s="34"/>
-      <c r="AX16" s="33"/>
+      <c r="AW16" s="35"/>
+      <c r="AX16" s="34"/>
       <c r="AY16" s="28"/>
       <c r="AZ16" s="28"/>
       <c r="BA16" s="28"/>
-      <c r="BB16" s="34"/>
+      <c r="BB16" s="35"/>
       <c r="BC16" s="0"/>
       <c r="BD16" s="0"/>
       <c r="BE16" s="0"/>
@@ -3019,209 +2931,209 @@
       <c r="A17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="39"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
       <c r="R17" s="28"/>
-      <c r="S17" s="34"/>
-      <c r="T17" s="33"/>
+      <c r="S17" s="35"/>
+      <c r="T17" s="34"/>
       <c r="U17" s="28"/>
       <c r="V17" s="28"/>
       <c r="W17" s="28"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="33"/>
+      <c r="X17" s="35"/>
+      <c r="Y17" s="34"/>
       <c r="Z17" s="28"/>
       <c r="AA17" s="28"/>
       <c r="AB17" s="28"/>
-      <c r="AC17" s="34"/>
-      <c r="AD17" s="33"/>
+      <c r="AC17" s="35"/>
+      <c r="AD17" s="34"/>
       <c r="AE17" s="28"/>
       <c r="AF17" s="28"/>
       <c r="AG17" s="28"/>
-      <c r="AH17" s="34"/>
-      <c r="AI17" s="33"/>
+      <c r="AH17" s="35"/>
+      <c r="AI17" s="34"/>
       <c r="AJ17" s="28"/>
       <c r="AK17" s="28"/>
       <c r="AL17" s="28"/>
-      <c r="AM17" s="34"/>
-      <c r="AN17" s="33"/>
+      <c r="AM17" s="35"/>
+      <c r="AN17" s="34"/>
       <c r="AO17" s="28"/>
       <c r="AP17" s="28"/>
       <c r="AQ17" s="28"/>
-      <c r="AR17" s="34"/>
-      <c r="AS17" s="33"/>
+      <c r="AR17" s="35"/>
+      <c r="AS17" s="34"/>
       <c r="AT17" s="28"/>
       <c r="AU17" s="28"/>
       <c r="AV17" s="28"/>
-      <c r="AW17" s="34"/>
-      <c r="AX17" s="33"/>
+      <c r="AW17" s="35"/>
+      <c r="AX17" s="34"/>
       <c r="AY17" s="28"/>
       <c r="AZ17" s="28"/>
       <c r="BA17" s="28"/>
-      <c r="BB17" s="34"/>
+      <c r="BB17" s="35"/>
     </row>
     <row r="18" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="30"/>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="33"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="N18" s="41"/>
       <c r="O18" s="28"/>
       <c r="P18" s="28"/>
       <c r="Q18" s="28"/>
       <c r="R18" s="28"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="33"/>
+      <c r="S18" s="35"/>
+      <c r="T18" s="34"/>
       <c r="U18" s="28"/>
       <c r="V18" s="28"/>
       <c r="W18" s="28"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="33"/>
+      <c r="X18" s="35"/>
+      <c r="Y18" s="34"/>
       <c r="Z18" s="28"/>
       <c r="AA18" s="28"/>
       <c r="AB18" s="28"/>
-      <c r="AC18" s="34"/>
-      <c r="AD18" s="33"/>
+      <c r="AC18" s="35"/>
+      <c r="AD18" s="34"/>
       <c r="AE18" s="28"/>
       <c r="AF18" s="28"/>
       <c r="AG18" s="28"/>
-      <c r="AH18" s="34"/>
-      <c r="AI18" s="33"/>
+      <c r="AH18" s="35"/>
+      <c r="AI18" s="34"/>
       <c r="AJ18" s="28"/>
       <c r="AK18" s="28"/>
       <c r="AL18" s="28"/>
-      <c r="AM18" s="34"/>
-      <c r="AN18" s="33"/>
+      <c r="AM18" s="35"/>
+      <c r="AN18" s="34"/>
       <c r="AO18" s="28"/>
       <c r="AP18" s="28"/>
       <c r="AQ18" s="28"/>
-      <c r="AR18" s="34"/>
-      <c r="AS18" s="33"/>
+      <c r="AR18" s="35"/>
+      <c r="AS18" s="34"/>
       <c r="AT18" s="28"/>
       <c r="AU18" s="28"/>
       <c r="AV18" s="28"/>
-      <c r="AW18" s="34"/>
-      <c r="AX18" s="33"/>
+      <c r="AW18" s="35"/>
+      <c r="AX18" s="34"/>
       <c r="AY18" s="28"/>
       <c r="AZ18" s="28"/>
       <c r="BA18" s="28"/>
-      <c r="BB18" s="34"/>
+      <c r="BB18" s="35"/>
     </row>
     <row r="19" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="30"/>
       <c r="B19" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="28"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="33"/>
+      <c r="S19" s="35"/>
+      <c r="T19" s="34"/>
       <c r="U19" s="28"/>
       <c r="V19" s="28"/>
       <c r="W19" s="28"/>
-      <c r="X19" s="34"/>
-      <c r="Y19" s="33"/>
+      <c r="X19" s="35"/>
+      <c r="Y19" s="34"/>
       <c r="Z19" s="28"/>
       <c r="AA19" s="28"/>
       <c r="AB19" s="28"/>
-      <c r="AC19" s="34"/>
-      <c r="AD19" s="33"/>
+      <c r="AC19" s="35"/>
+      <c r="AD19" s="34"/>
       <c r="AE19" s="28"/>
       <c r="AF19" s="28"/>
       <c r="AG19" s="28"/>
-      <c r="AH19" s="34"/>
-      <c r="AI19" s="33"/>
+      <c r="AH19" s="35"/>
+      <c r="AI19" s="34"/>
       <c r="AJ19" s="28"/>
       <c r="AK19" s="28"/>
       <c r="AL19" s="28"/>
-      <c r="AM19" s="34"/>
-      <c r="AN19" s="33"/>
+      <c r="AM19" s="35"/>
+      <c r="AN19" s="34"/>
       <c r="AO19" s="28"/>
       <c r="AP19" s="28"/>
       <c r="AQ19" s="28"/>
-      <c r="AR19" s="34"/>
-      <c r="AS19" s="33"/>
+      <c r="AR19" s="35"/>
+      <c r="AS19" s="34"/>
       <c r="AT19" s="28"/>
       <c r="AU19" s="28"/>
       <c r="AV19" s="28"/>
-      <c r="AW19" s="34"/>
-      <c r="AX19" s="33"/>
+      <c r="AW19" s="35"/>
+      <c r="AX19" s="34"/>
       <c r="AY19" s="28"/>
       <c r="AZ19" s="28"/>
       <c r="BA19" s="28"/>
-      <c r="BB19" s="34"/>
+      <c r="BB19" s="35"/>
     </row>
     <row r="20" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="30"/>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="43"/>
-      <c r="E20" s="33"/>
+      <c r="E20" s="34"/>
       <c r="F20" s="28"/>
-      <c r="G20" s="41"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="28"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="33"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="34"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="33"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="28"/>
       <c r="Q20" s="28"/>
       <c r="R20" s="28"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="33"/>
+      <c r="S20" s="35"/>
+      <c r="T20" s="34"/>
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
       <c r="W20" s="28"/>
@@ -3235,27 +3147,27 @@
       <c r="AE20" s="28"/>
       <c r="AF20" s="29"/>
       <c r="AG20" s="28"/>
-      <c r="AH20" s="34"/>
-      <c r="AI20" s="33"/>
+      <c r="AH20" s="35"/>
+      <c r="AI20" s="34"/>
       <c r="AJ20" s="28"/>
       <c r="AK20" s="28"/>
       <c r="AL20" s="28"/>
-      <c r="AM20" s="34"/>
-      <c r="AN20" s="33"/>
+      <c r="AM20" s="35"/>
+      <c r="AN20" s="34"/>
       <c r="AO20" s="28"/>
       <c r="AP20" s="28"/>
       <c r="AQ20" s="28"/>
-      <c r="AR20" s="34"/>
-      <c r="AS20" s="33"/>
+      <c r="AR20" s="35"/>
+      <c r="AS20" s="34"/>
       <c r="AT20" s="28"/>
       <c r="AU20" s="28"/>
       <c r="AV20" s="28"/>
-      <c r="AW20" s="34"/>
-      <c r="AX20" s="33"/>
+      <c r="AW20" s="35"/>
+      <c r="AX20" s="34"/>
       <c r="AY20" s="28"/>
       <c r="AZ20" s="28"/>
       <c r="BA20" s="28"/>
-      <c r="BB20" s="34"/>
+      <c r="BB20" s="35"/>
       <c r="BC20" s="29"/>
       <c r="BD20" s="29"/>
       <c r="BE20" s="29"/>
@@ -3265,1222 +3177,1222 @@
       <c r="A21" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="32" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="47"/>
       <c r="E21" s="48"/>
-      <c r="F21" s="49"/>
+      <c r="F21" s="41"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="33"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="34"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="33"/>
+      <c r="N21" s="35"/>
+      <c r="O21" s="34"/>
       <c r="P21" s="28"/>
       <c r="Q21" s="28"/>
       <c r="R21" s="28"/>
-      <c r="S21" s="34"/>
-      <c r="T21" s="33"/>
+      <c r="S21" s="35"/>
+      <c r="T21" s="34"/>
       <c r="U21" s="28"/>
       <c r="V21" s="28"/>
       <c r="W21" s="28"/>
-      <c r="X21" s="34"/>
-      <c r="Y21" s="33"/>
+      <c r="X21" s="35"/>
+      <c r="Y21" s="34"/>
       <c r="Z21" s="28"/>
       <c r="AA21" s="28"/>
       <c r="AB21" s="28"/>
-      <c r="AC21" s="34"/>
-      <c r="AD21" s="33"/>
+      <c r="AC21" s="35"/>
+      <c r="AD21" s="34"/>
       <c r="AE21" s="28"/>
       <c r="AG21" s="28"/>
-      <c r="AH21" s="34"/>
-      <c r="AJ21" s="50"/>
-      <c r="AK21" s="50"/>
-      <c r="AL21" s="50"/>
-      <c r="AM21" s="50"/>
-      <c r="AN21" s="50"/>
-      <c r="AO21" s="50"/>
+      <c r="AH21" s="35"/>
+      <c r="AJ21" s="49"/>
+      <c r="AK21" s="49"/>
+      <c r="AL21" s="49"/>
+      <c r="AM21" s="49"/>
+      <c r="AN21" s="49"/>
+      <c r="AO21" s="49"/>
       <c r="AP21" s="28"/>
-      <c r="AQ21" s="50"/>
-      <c r="AR21" s="50"/>
-      <c r="AS21" s="50"/>
-      <c r="AT21" s="50"/>
-      <c r="AU21" s="50"/>
-      <c r="AV21" s="50"/>
-      <c r="AW21" s="50"/>
-      <c r="AX21" s="33"/>
+      <c r="AQ21" s="49"/>
+      <c r="AR21" s="49"/>
+      <c r="AS21" s="49"/>
+      <c r="AT21" s="49"/>
+      <c r="AU21" s="49"/>
+      <c r="AV21" s="49"/>
+      <c r="AW21" s="49"/>
+      <c r="AX21" s="34"/>
       <c r="AY21" s="28"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="28"/>
-      <c r="BB21" s="34"/>
+      <c r="BB21" s="35"/>
     </row>
     <row r="22" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="33"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="34"/>
       <c r="F22" s="28"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="33"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="34"/>
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="28"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="53"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="28"/>
-      <c r="S22" s="34"/>
-      <c r="T22" s="33"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="34"/>
       <c r="U22" s="28"/>
       <c r="V22" s="28"/>
       <c r="W22" s="28"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="33"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="34"/>
       <c r="Z22" s="28"/>
       <c r="AA22" s="28"/>
       <c r="AB22" s="28"/>
-      <c r="AC22" s="34"/>
-      <c r="AD22" s="33"/>
+      <c r="AC22" s="35"/>
+      <c r="AD22" s="34"/>
       <c r="AE22" s="28"/>
       <c r="AG22" s="28"/>
-      <c r="AH22" s="34"/>
-      <c r="AJ22" s="50"/>
-      <c r="AK22" s="50"/>
-      <c r="AL22" s="50"/>
-      <c r="AM22" s="50"/>
-      <c r="AN22" s="50"/>
-      <c r="AO22" s="50"/>
+      <c r="AH22" s="35"/>
+      <c r="AJ22" s="49"/>
+      <c r="AK22" s="49"/>
+      <c r="AL22" s="49"/>
+      <c r="AM22" s="49"/>
+      <c r="AN22" s="49"/>
+      <c r="AO22" s="49"/>
       <c r="AP22" s="28"/>
-      <c r="AQ22" s="50"/>
-      <c r="AR22" s="50"/>
-      <c r="AS22" s="50"/>
-      <c r="AT22" s="50"/>
-      <c r="AU22" s="50"/>
-      <c r="AV22" s="50"/>
-      <c r="AW22" s="50"/>
-      <c r="AX22" s="33"/>
+      <c r="AQ22" s="49"/>
+      <c r="AR22" s="49"/>
+      <c r="AS22" s="49"/>
+      <c r="AT22" s="49"/>
+      <c r="AU22" s="49"/>
+      <c r="AV22" s="49"/>
+      <c r="AW22" s="49"/>
+      <c r="AX22" s="34"/>
       <c r="AY22" s="28"/>
       <c r="AZ22" s="28"/>
       <c r="BA22" s="28"/>
-      <c r="BB22" s="34"/>
+      <c r="BB22" s="35"/>
     </row>
     <row r="23" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="33"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="34"/>
       <c r="F23" s="28"/>
       <c r="G23" s="28"/>
       <c r="H23" s="28"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="33"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="34"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="28"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="53"/>
       <c r="Q23" s="28"/>
       <c r="R23" s="28"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="33"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="34"/>
       <c r="U23" s="28"/>
       <c r="V23" s="28"/>
       <c r="W23" s="28"/>
-      <c r="X23" s="34"/>
-      <c r="Y23" s="33"/>
+      <c r="X23" s="35"/>
+      <c r="Y23" s="34"/>
       <c r="Z23" s="28"/>
       <c r="AA23" s="28"/>
       <c r="AB23" s="28"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="33"/>
+      <c r="AC23" s="35"/>
+      <c r="AD23" s="34"/>
       <c r="AE23" s="28"/>
       <c r="AG23" s="28"/>
-      <c r="AH23" s="34"/>
-      <c r="AJ23" s="50"/>
-      <c r="AK23" s="50"/>
-      <c r="AL23" s="50"/>
-      <c r="AM23" s="50"/>
-      <c r="AN23" s="50"/>
-      <c r="AO23" s="50"/>
+      <c r="AH23" s="35"/>
+      <c r="AJ23" s="49"/>
+      <c r="AK23" s="49"/>
+      <c r="AL23" s="49"/>
+      <c r="AM23" s="49"/>
+      <c r="AN23" s="49"/>
+      <c r="AO23" s="49"/>
       <c r="AP23" s="28"/>
-      <c r="AQ23" s="50"/>
-      <c r="AR23" s="50"/>
-      <c r="AS23" s="50"/>
-      <c r="AT23" s="50"/>
-      <c r="AU23" s="50"/>
-      <c r="AV23" s="50"/>
-      <c r="AW23" s="50"/>
-      <c r="AX23" s="33"/>
+      <c r="AQ23" s="49"/>
+      <c r="AR23" s="49"/>
+      <c r="AS23" s="49"/>
+      <c r="AT23" s="49"/>
+      <c r="AU23" s="49"/>
+      <c r="AV23" s="49"/>
+      <c r="AW23" s="49"/>
+      <c r="AX23" s="34"/>
       <c r="AY23" s="28"/>
       <c r="AZ23" s="28"/>
       <c r="BA23" s="28"/>
-      <c r="BB23" s="34"/>
+      <c r="BB23" s="35"/>
     </row>
     <row r="24" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="33"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="34"/>
       <c r="F24" s="28"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="33"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="52"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="53"/>
       <c r="Q24" s="28"/>
       <c r="R24" s="28"/>
-      <c r="S24" s="34"/>
-      <c r="T24" s="33"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="34"/>
       <c r="U24" s="28"/>
       <c r="V24" s="28"/>
       <c r="W24" s="28"/>
-      <c r="X24" s="34"/>
-      <c r="Y24" s="33"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="34"/>
       <c r="Z24" s="28"/>
       <c r="AA24" s="28"/>
       <c r="AB24" s="28"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="33"/>
+      <c r="AC24" s="35"/>
+      <c r="AD24" s="34"/>
       <c r="AE24" s="28"/>
       <c r="AG24" s="28"/>
-      <c r="AH24" s="34"/>
-      <c r="AJ24" s="50"/>
-      <c r="AK24" s="50"/>
-      <c r="AL24" s="50"/>
-      <c r="AM24" s="50"/>
-      <c r="AN24" s="50"/>
-      <c r="AO24" s="50"/>
+      <c r="AH24" s="35"/>
+      <c r="AJ24" s="49"/>
+      <c r="AK24" s="49"/>
+      <c r="AL24" s="49"/>
+      <c r="AM24" s="49"/>
+      <c r="AN24" s="49"/>
+      <c r="AO24" s="49"/>
       <c r="AP24" s="28"/>
-      <c r="AQ24" s="50"/>
-      <c r="AR24" s="50"/>
-      <c r="AS24" s="50"/>
-      <c r="AT24" s="50"/>
-      <c r="AU24" s="50"/>
-      <c r="AV24" s="50"/>
-      <c r="AW24" s="50"/>
-      <c r="AX24" s="33"/>
+      <c r="AQ24" s="49"/>
+      <c r="AR24" s="49"/>
+      <c r="AS24" s="49"/>
+      <c r="AT24" s="49"/>
+      <c r="AU24" s="49"/>
+      <c r="AV24" s="49"/>
+      <c r="AW24" s="49"/>
+      <c r="AX24" s="34"/>
       <c r="AY24" s="28"/>
       <c r="AZ24" s="28"/>
       <c r="BA24" s="28"/>
-      <c r="BB24" s="34"/>
+      <c r="BB24" s="35"/>
     </row>
     <row r="25" customFormat="false" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="33"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="34"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="33"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="34"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="33"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="34"/>
       <c r="P25" s="28"/>
       <c r="Q25" s="28"/>
-      <c r="R25" s="52"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="33"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="34"/>
       <c r="U25" s="28"/>
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
-      <c r="X25" s="34"/>
-      <c r="Y25" s="33"/>
+      <c r="X25" s="35"/>
+      <c r="Y25" s="34"/>
       <c r="Z25" s="28"/>
       <c r="AA25" s="28"/>
       <c r="AB25" s="28"/>
-      <c r="AC25" s="34"/>
-      <c r="AD25" s="33"/>
+      <c r="AC25" s="35"/>
+      <c r="AD25" s="34"/>
       <c r="AE25" s="28"/>
       <c r="AF25" s="28"/>
       <c r="AG25" s="28"/>
-      <c r="AH25" s="34"/>
-      <c r="AJ25" s="50"/>
-      <c r="AK25" s="50"/>
-      <c r="AL25" s="50"/>
-      <c r="AM25" s="50"/>
-      <c r="AN25" s="50"/>
-      <c r="AO25" s="50"/>
+      <c r="AH25" s="35"/>
+      <c r="AJ25" s="49"/>
+      <c r="AK25" s="49"/>
+      <c r="AL25" s="49"/>
+      <c r="AM25" s="49"/>
+      <c r="AN25" s="49"/>
+      <c r="AO25" s="49"/>
       <c r="AP25" s="28"/>
-      <c r="AQ25" s="50"/>
-      <c r="AR25" s="50"/>
-      <c r="AS25" s="50"/>
-      <c r="AT25" s="50"/>
-      <c r="AU25" s="50"/>
-      <c r="AV25" s="50"/>
-      <c r="AW25" s="50"/>
-      <c r="AX25" s="33"/>
+      <c r="AQ25" s="49"/>
+      <c r="AR25" s="49"/>
+      <c r="AS25" s="49"/>
+      <c r="AT25" s="49"/>
+      <c r="AU25" s="49"/>
+      <c r="AV25" s="49"/>
+      <c r="AW25" s="49"/>
+      <c r="AX25" s="34"/>
       <c r="AY25" s="28"/>
       <c r="AZ25" s="28"/>
       <c r="BA25" s="28"/>
-      <c r="BB25" s="34"/>
+      <c r="BB25" s="35"/>
     </row>
     <row r="26" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="53"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="53"/>
-      <c r="T26" s="53"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="53"/>
-      <c r="W26" s="53"/>
-      <c r="X26" s="53"/>
-      <c r="Y26" s="33"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="54"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="54"/>
+      <c r="N26" s="54"/>
+      <c r="O26" s="54"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="54"/>
+      <c r="S26" s="54"/>
+      <c r="T26" s="54"/>
+      <c r="U26" s="54"/>
+      <c r="V26" s="54"/>
+      <c r="W26" s="54"/>
+      <c r="X26" s="54"/>
+      <c r="Y26" s="34"/>
       <c r="Z26" s="28"/>
       <c r="AA26" s="28"/>
       <c r="AB26" s="28"/>
-      <c r="AC26" s="34"/>
-      <c r="AD26" s="33"/>
+      <c r="AC26" s="35"/>
+      <c r="AD26" s="34"/>
       <c r="AE26" s="28"/>
       <c r="AF26" s="28"/>
       <c r="AG26" s="28"/>
-      <c r="AH26" s="34"/>
-      <c r="AI26" s="33"/>
+      <c r="AH26" s="35"/>
+      <c r="AI26" s="34"/>
       <c r="AJ26" s="28"/>
       <c r="AK26" s="28"/>
       <c r="AL26" s="28"/>
-      <c r="AM26" s="34"/>
-      <c r="AN26" s="33"/>
+      <c r="AM26" s="35"/>
+      <c r="AN26" s="34"/>
       <c r="AO26" s="28"/>
       <c r="AP26" s="28"/>
       <c r="AQ26" s="28"/>
-      <c r="AR26" s="34"/>
-      <c r="AS26" s="33"/>
+      <c r="AR26" s="35"/>
+      <c r="AS26" s="34"/>
       <c r="AT26" s="28"/>
       <c r="AU26" s="28"/>
       <c r="AV26" s="28"/>
-      <c r="AW26" s="34"/>
-      <c r="AX26" s="33"/>
+      <c r="AW26" s="35"/>
+      <c r="AX26" s="34"/>
       <c r="AY26" s="28"/>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="28"/>
-      <c r="BB26" s="34"/>
+      <c r="BB26" s="35"/>
     </row>
     <row r="27" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="55"/>
-      <c r="T27" s="55"/>
-      <c r="U27" s="56"/>
-      <c r="V27" s="55"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="33"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="57"/>
+      <c r="V27" s="56"/>
+      <c r="W27" s="56"/>
+      <c r="X27" s="50"/>
+      <c r="Y27" s="34"/>
       <c r="Z27" s="28"/>
       <c r="AA27" s="28"/>
       <c r="AB27" s="28"/>
-      <c r="AC27" s="34"/>
-      <c r="AD27" s="33"/>
+      <c r="AC27" s="35"/>
+      <c r="AD27" s="34"/>
       <c r="AE27" s="28"/>
       <c r="AF27" s="28"/>
       <c r="AG27" s="28"/>
-      <c r="AH27" s="34"/>
-      <c r="AI27" s="33"/>
+      <c r="AH27" s="35"/>
+      <c r="AI27" s="34"/>
       <c r="AJ27" s="28"/>
       <c r="AK27" s="28"/>
       <c r="AL27" s="28"/>
-      <c r="AM27" s="34"/>
-      <c r="AN27" s="33"/>
+      <c r="AM27" s="35"/>
+      <c r="AN27" s="34"/>
       <c r="AO27" s="28"/>
       <c r="AP27" s="28"/>
       <c r="AQ27" s="28"/>
-      <c r="AR27" s="34"/>
-      <c r="AS27" s="33"/>
+      <c r="AR27" s="35"/>
+      <c r="AS27" s="34"/>
       <c r="AT27" s="28"/>
       <c r="AU27" s="28"/>
       <c r="AV27" s="28"/>
-      <c r="AW27" s="34"/>
-      <c r="AX27" s="33"/>
+      <c r="AW27" s="35"/>
+      <c r="AX27" s="34"/>
       <c r="AY27" s="28"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="28"/>
-      <c r="BB27" s="34"/>
+      <c r="BB27" s="35"/>
     </row>
     <row r="28" customFormat="false" ht="20.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="46"/>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="33"/>
-      <c r="Z28" s="52"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="56"/>
+      <c r="W28" s="56"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="53"/>
       <c r="AA28" s="28"/>
       <c r="AB28" s="28"/>
-      <c r="AC28" s="34"/>
-      <c r="AD28" s="33"/>
+      <c r="AC28" s="35"/>
+      <c r="AD28" s="34"/>
       <c r="AE28" s="28"/>
       <c r="AF28" s="28"/>
       <c r="AG28" s="28"/>
-      <c r="AH28" s="34"/>
-      <c r="AI28" s="33"/>
+      <c r="AH28" s="35"/>
+      <c r="AI28" s="34"/>
       <c r="AJ28" s="28"/>
       <c r="AK28" s="28"/>
       <c r="AL28" s="28"/>
-      <c r="AM28" s="34"/>
-      <c r="AN28" s="33"/>
+      <c r="AM28" s="35"/>
+      <c r="AN28" s="34"/>
       <c r="AO28" s="28"/>
       <c r="AP28" s="28"/>
       <c r="AQ28" s="28"/>
-      <c r="AR28" s="34"/>
-      <c r="AS28" s="33"/>
+      <c r="AR28" s="35"/>
+      <c r="AS28" s="34"/>
       <c r="AT28" s="28"/>
       <c r="AU28" s="28"/>
       <c r="AV28" s="28"/>
-      <c r="AW28" s="34"/>
-      <c r="AX28" s="33"/>
+      <c r="AW28" s="35"/>
+      <c r="AX28" s="34"/>
       <c r="AY28" s="28"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="28"/>
-      <c r="BB28" s="34"/>
+      <c r="BB28" s="35"/>
     </row>
     <row r="29" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="46"/>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="55"/>
-      <c r="T29" s="55"/>
-      <c r="U29" s="55"/>
-      <c r="V29" s="55"/>
-      <c r="W29" s="55"/>
-      <c r="X29" s="51"/>
-      <c r="Y29" s="33"/>
-      <c r="Z29" s="52"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+      <c r="S29" s="56"/>
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="V29" s="56"/>
+      <c r="W29" s="56"/>
+      <c r="X29" s="50"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="53"/>
       <c r="AA29" s="28"/>
       <c r="AB29" s="28"/>
-      <c r="AC29" s="34"/>
-      <c r="AD29" s="33"/>
+      <c r="AC29" s="35"/>
+      <c r="AD29" s="34"/>
       <c r="AE29" s="28"/>
       <c r="AF29" s="28"/>
       <c r="AG29" s="28"/>
-      <c r="AH29" s="34"/>
-      <c r="AI29" s="33"/>
+      <c r="AH29" s="35"/>
+      <c r="AI29" s="34"/>
       <c r="AJ29" s="28"/>
       <c r="AK29" s="28"/>
       <c r="AL29" s="28"/>
-      <c r="AM29" s="34"/>
-      <c r="AN29" s="33"/>
+      <c r="AM29" s="35"/>
+      <c r="AN29" s="34"/>
       <c r="AO29" s="28"/>
       <c r="AP29" s="28"/>
       <c r="AQ29" s="28"/>
-      <c r="AR29" s="34"/>
-      <c r="AS29" s="33"/>
+      <c r="AR29" s="35"/>
+      <c r="AS29" s="34"/>
       <c r="AT29" s="28"/>
       <c r="AU29" s="28"/>
       <c r="AV29" s="28"/>
-      <c r="AW29" s="34"/>
-      <c r="AX29" s="33"/>
+      <c r="AW29" s="35"/>
+      <c r="AX29" s="34"/>
       <c r="AY29" s="28"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="28"/>
-      <c r="BB29" s="34"/>
+      <c r="BB29" s="35"/>
     </row>
     <row r="30" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="46"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="34"/>
-      <c r="E30" s="33"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="34"/>
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="36"/>
-      <c r="N30" s="37"/>
-      <c r="O30" s="33"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="34"/>
       <c r="P30" s="28"/>
       <c r="Q30" s="28"/>
       <c r="R30" s="28"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="33"/>
+      <c r="S30" s="35"/>
+      <c r="T30" s="34"/>
       <c r="U30" s="28"/>
       <c r="V30" s="28"/>
       <c r="W30" s="28"/>
-      <c r="X30" s="34"/>
-      <c r="Y30" s="33"/>
+      <c r="X30" s="35"/>
+      <c r="Y30" s="34"/>
       <c r="Z30" s="28"/>
       <c r="AA30" s="28"/>
       <c r="AB30" s="28"/>
-      <c r="AC30" s="34"/>
-      <c r="AD30" s="58"/>
+      <c r="AC30" s="35"/>
+      <c r="AD30" s="59"/>
       <c r="AE30" s="28"/>
       <c r="AF30" s="28"/>
       <c r="AG30" s="28"/>
-      <c r="AH30" s="34"/>
-      <c r="AI30" s="33"/>
+      <c r="AH30" s="35"/>
+      <c r="AI30" s="34"/>
       <c r="AJ30" s="28"/>
       <c r="AK30" s="28"/>
       <c r="AL30" s="28"/>
-      <c r="AM30" s="34"/>
-      <c r="AN30" s="33"/>
+      <c r="AM30" s="35"/>
+      <c r="AN30" s="34"/>
       <c r="AO30" s="28"/>
       <c r="AP30" s="28"/>
       <c r="AQ30" s="28"/>
-      <c r="AR30" s="34"/>
-      <c r="AS30" s="33"/>
+      <c r="AR30" s="35"/>
+      <c r="AS30" s="34"/>
       <c r="AT30" s="28"/>
       <c r="AU30" s="28"/>
       <c r="AV30" s="28"/>
-      <c r="AW30" s="34"/>
-      <c r="AX30" s="33"/>
+      <c r="AW30" s="35"/>
+      <c r="AX30" s="34"/>
       <c r="AY30" s="28"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="28"/>
-      <c r="BB30" s="34"/>
+      <c r="BB30" s="35"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="46"/>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="57" t="s">
+      <c r="C31" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="33"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="34"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="36"/>
-      <c r="L31" s="36"/>
-      <c r="M31" s="36"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="33"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="37"/>
+      <c r="L31" s="37"/>
+      <c r="M31" s="37"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="34"/>
       <c r="P31" s="28"/>
       <c r="Q31" s="28"/>
       <c r="R31" s="28"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="58"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="59"/>
       <c r="U31" s="28"/>
       <c r="V31" s="28"/>
       <c r="W31" s="28"/>
-      <c r="X31" s="34"/>
-      <c r="Y31" s="33"/>
+      <c r="X31" s="35"/>
+      <c r="Y31" s="34"/>
       <c r="Z31" s="28"/>
       <c r="AA31" s="28"/>
       <c r="AB31" s="28"/>
-      <c r="AC31" s="34"/>
-      <c r="AD31" s="33"/>
+      <c r="AC31" s="35"/>
+      <c r="AD31" s="34"/>
       <c r="AE31" s="28"/>
       <c r="AF31" s="28"/>
       <c r="AG31" s="28"/>
-      <c r="AH31" s="34"/>
-      <c r="AI31" s="33"/>
+      <c r="AH31" s="35"/>
+      <c r="AI31" s="34"/>
       <c r="AJ31" s="28"/>
       <c r="AK31" s="28"/>
       <c r="AL31" s="28"/>
-      <c r="AM31" s="34"/>
-      <c r="AN31" s="33"/>
+      <c r="AM31" s="35"/>
+      <c r="AN31" s="34"/>
       <c r="AO31" s="28"/>
       <c r="AP31" s="28"/>
       <c r="AQ31" s="28"/>
-      <c r="AR31" s="34"/>
-      <c r="AS31" s="33"/>
+      <c r="AR31" s="35"/>
+      <c r="AS31" s="34"/>
       <c r="AT31" s="28"/>
       <c r="AU31" s="28"/>
       <c r="AV31" s="28"/>
-      <c r="AW31" s="34"/>
-      <c r="AX31" s="33"/>
+      <c r="AW31" s="35"/>
+      <c r="AX31" s="34"/>
       <c r="AY31" s="28"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="28"/>
-      <c r="BB31" s="34"/>
+      <c r="BB31" s="35"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="33"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="34"/>
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="36"/>
-      <c r="M32" s="36"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="33"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="34"/>
       <c r="P32" s="28"/>
       <c r="Q32" s="28"/>
       <c r="R32" s="28"/>
-      <c r="S32" s="34"/>
-      <c r="T32" s="58"/>
+      <c r="S32" s="35"/>
+      <c r="T32" s="59"/>
       <c r="U32" s="28"/>
       <c r="V32" s="28"/>
       <c r="W32" s="28"/>
-      <c r="X32" s="34"/>
-      <c r="Y32" s="33"/>
+      <c r="X32" s="35"/>
+      <c r="Y32" s="34"/>
       <c r="Z32" s="28"/>
       <c r="AA32" s="28"/>
       <c r="AB32" s="28"/>
-      <c r="AC32" s="34"/>
-      <c r="AD32" s="33"/>
+      <c r="AC32" s="35"/>
+      <c r="AD32" s="34"/>
       <c r="AE32" s="28"/>
       <c r="AF32" s="28"/>
       <c r="AG32" s="28"/>
-      <c r="AH32" s="34"/>
-      <c r="AI32" s="33"/>
+      <c r="AH32" s="35"/>
+      <c r="AI32" s="34"/>
       <c r="AJ32" s="28"/>
       <c r="AK32" s="28"/>
       <c r="AL32" s="28"/>
-      <c r="AM32" s="34"/>
-      <c r="AN32" s="33"/>
+      <c r="AM32" s="35"/>
+      <c r="AN32" s="34"/>
       <c r="AO32" s="28"/>
       <c r="AP32" s="28"/>
       <c r="AQ32" s="28"/>
-      <c r="AR32" s="34"/>
-      <c r="AS32" s="33"/>
+      <c r="AR32" s="35"/>
+      <c r="AS32" s="34"/>
       <c r="AT32" s="28"/>
       <c r="AU32" s="28"/>
       <c r="AV32" s="28"/>
-      <c r="AW32" s="34"/>
-      <c r="AX32" s="33"/>
+      <c r="AW32" s="35"/>
+      <c r="AX32" s="34"/>
       <c r="AY32" s="28"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="28"/>
-      <c r="BB32" s="34"/>
+      <c r="BB32" s="35"/>
     </row>
     <row r="33" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="33"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="34"/>
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="36"/>
-      <c r="M33" s="36"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="33"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="37"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="34"/>
       <c r="P33" s="28"/>
       <c r="Q33" s="28"/>
       <c r="R33" s="28"/>
-      <c r="S33" s="34"/>
-      <c r="T33" s="33"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="34"/>
       <c r="U33" s="28"/>
       <c r="V33" s="28"/>
       <c r="W33" s="28"/>
-      <c r="X33" s="34"/>
-      <c r="Y33" s="33"/>
+      <c r="X33" s="35"/>
+      <c r="Y33" s="34"/>
       <c r="Z33" s="28"/>
       <c r="AA33" s="28"/>
       <c r="AB33" s="28"/>
-      <c r="AC33" s="34"/>
-      <c r="AD33" s="33"/>
+      <c r="AC33" s="35"/>
+      <c r="AD33" s="34"/>
       <c r="AE33" s="28"/>
       <c r="AF33" s="28"/>
       <c r="AG33" s="28"/>
-      <c r="AH33" s="59"/>
-      <c r="AI33" s="33"/>
+      <c r="AH33" s="60"/>
+      <c r="AI33" s="34"/>
       <c r="AJ33" s="28"/>
       <c r="AK33" s="28"/>
       <c r="AL33" s="28"/>
-      <c r="AM33" s="34"/>
-      <c r="AN33" s="33"/>
+      <c r="AM33" s="35"/>
+      <c r="AN33" s="34"/>
       <c r="AO33" s="28"/>
       <c r="AP33" s="28"/>
       <c r="AQ33" s="28"/>
-      <c r="AR33" s="34"/>
-      <c r="AS33" s="33"/>
+      <c r="AR33" s="35"/>
+      <c r="AS33" s="34"/>
       <c r="AT33" s="28"/>
       <c r="AU33" s="28"/>
       <c r="AV33" s="28"/>
-      <c r="AW33" s="34"/>
-      <c r="AX33" s="33"/>
+      <c r="AW33" s="35"/>
+      <c r="AX33" s="34"/>
       <c r="AY33" s="28"/>
       <c r="AZ33" s="28"/>
       <c r="BA33" s="28"/>
-      <c r="BB33" s="34"/>
+      <c r="BB33" s="35"/>
     </row>
     <row r="34" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="C34" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
       <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="33"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="36"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="38"/>
+      <c r="O34" s="34"/>
       <c r="P34" s="28"/>
       <c r="Q34" s="28"/>
       <c r="R34" s="28"/>
-      <c r="S34" s="34"/>
-      <c r="T34" s="33"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="34"/>
       <c r="U34" s="28"/>
       <c r="V34" s="28"/>
       <c r="W34" s="28"/>
-      <c r="X34" s="34"/>
-      <c r="Y34" s="33"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="34"/>
       <c r="Z34" s="28"/>
       <c r="AA34" s="28"/>
       <c r="AB34" s="28"/>
-      <c r="AC34" s="59"/>
-      <c r="AD34" s="33"/>
+      <c r="AC34" s="60"/>
+      <c r="AD34" s="34"/>
       <c r="AE34" s="28"/>
       <c r="AF34" s="28"/>
       <c r="AG34" s="28"/>
-      <c r="AH34" s="34"/>
-      <c r="AI34" s="33"/>
+      <c r="AH34" s="35"/>
+      <c r="AI34" s="34"/>
       <c r="AJ34" s="28"/>
       <c r="AK34" s="28"/>
       <c r="AL34" s="28"/>
-      <c r="AM34" s="34"/>
-      <c r="AN34" s="33"/>
+      <c r="AM34" s="35"/>
+      <c r="AN34" s="34"/>
       <c r="AO34" s="28"/>
       <c r="AP34" s="28"/>
       <c r="AQ34" s="28"/>
-      <c r="AR34" s="34"/>
-      <c r="AS34" s="33"/>
+      <c r="AR34" s="35"/>
+      <c r="AS34" s="34"/>
       <c r="AT34" s="28"/>
       <c r="AU34" s="28"/>
       <c r="AV34" s="28"/>
-      <c r="AW34" s="34"/>
-      <c r="AX34" s="33"/>
+      <c r="AW34" s="35"/>
+      <c r="AX34" s="34"/>
       <c r="AY34" s="28"/>
       <c r="AZ34" s="28"/>
       <c r="BA34" s="28"/>
-      <c r="BB34" s="34"/>
+      <c r="BB34" s="35"/>
     </row>
     <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="33"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="34"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="36"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="33"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="37"/>
+      <c r="L35" s="37"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="34"/>
       <c r="P35" s="28"/>
       <c r="Q35" s="28"/>
       <c r="R35" s="28"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="33"/>
+      <c r="S35" s="35"/>
+      <c r="T35" s="34"/>
       <c r="U35" s="28"/>
       <c r="V35" s="28"/>
       <c r="W35" s="28"/>
-      <c r="X35" s="34"/>
-      <c r="Y35" s="33"/>
-      <c r="Z35" s="52"/>
+      <c r="X35" s="35"/>
+      <c r="Y35" s="34"/>
+      <c r="Z35" s="53"/>
       <c r="AA35" s="28"/>
       <c r="AB35" s="28"/>
-      <c r="AC35" s="34"/>
-      <c r="AD35" s="33"/>
+      <c r="AC35" s="35"/>
+      <c r="AD35" s="34"/>
       <c r="AE35" s="28"/>
       <c r="AF35" s="28"/>
       <c r="AG35" s="28"/>
-      <c r="AH35" s="34"/>
-      <c r="AI35" s="33"/>
+      <c r="AH35" s="35"/>
+      <c r="AI35" s="34"/>
       <c r="AJ35" s="28"/>
       <c r="AK35" s="28"/>
       <c r="AL35" s="28"/>
-      <c r="AM35" s="34"/>
-      <c r="AN35" s="33"/>
+      <c r="AM35" s="35"/>
+      <c r="AN35" s="34"/>
       <c r="AO35" s="28"/>
       <c r="AP35" s="28"/>
       <c r="AQ35" s="28"/>
-      <c r="AR35" s="34"/>
-      <c r="AS35" s="33"/>
+      <c r="AR35" s="35"/>
+      <c r="AS35" s="34"/>
       <c r="AT35" s="28"/>
       <c r="AU35" s="28"/>
       <c r="AV35" s="28"/>
-      <c r="AW35" s="34"/>
-      <c r="AX35" s="33"/>
+      <c r="AW35" s="35"/>
+      <c r="AX35" s="34"/>
       <c r="AY35" s="28"/>
       <c r="AZ35" s="28"/>
       <c r="BA35" s="28"/>
-      <c r="BB35" s="34"/>
+      <c r="BB35" s="35"/>
     </row>
     <row r="36" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="32" t="s">
         <v>59</v>
       </c>
       <c r="C36" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="36"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="33"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="37"/>
+      <c r="L36" s="37"/>
+      <c r="M36" s="37"/>
+      <c r="N36" s="38"/>
+      <c r="O36" s="34"/>
       <c r="P36" s="28"/>
       <c r="Q36" s="28"/>
       <c r="R36" s="28"/>
-      <c r="S36" s="34"/>
-      <c r="T36" s="33"/>
+      <c r="S36" s="35"/>
+      <c r="T36" s="34"/>
       <c r="U36" s="28"/>
       <c r="V36" s="28"/>
       <c r="W36" s="28"/>
-      <c r="X36" s="34"/>
-      <c r="Y36" s="33"/>
+      <c r="X36" s="35"/>
+      <c r="Y36" s="34"/>
       <c r="Z36" s="28"/>
       <c r="AA36" s="28"/>
       <c r="AB36" s="28"/>
-      <c r="AC36" s="34"/>
-      <c r="AD36" s="33"/>
+      <c r="AC36" s="35"/>
+      <c r="AD36" s="34"/>
       <c r="AE36" s="28"/>
       <c r="AF36" s="28"/>
       <c r="AG36" s="28"/>
-      <c r="AH36" s="34"/>
-      <c r="AI36" s="33"/>
+      <c r="AH36" s="35"/>
+      <c r="AI36" s="34"/>
       <c r="AJ36" s="28"/>
       <c r="AK36" s="28"/>
       <c r="AL36" s="28"/>
-      <c r="AM36" s="34"/>
-      <c r="AN36" s="58"/>
+      <c r="AM36" s="35"/>
+      <c r="AN36" s="59"/>
       <c r="AO36" s="28"/>
       <c r="AP36" s="28"/>
       <c r="AQ36" s="28"/>
-      <c r="AR36" s="34"/>
-      <c r="AS36" s="33"/>
+      <c r="AR36" s="35"/>
+      <c r="AS36" s="34"/>
       <c r="AT36" s="28"/>
       <c r="AU36" s="28"/>
       <c r="AV36" s="28"/>
-      <c r="AW36" s="34"/>
-      <c r="AX36" s="33"/>
+      <c r="AW36" s="35"/>
+      <c r="AX36" s="34"/>
       <c r="AY36" s="28"/>
       <c r="AZ36" s="28"/>
       <c r="BA36" s="28"/>
-      <c r="BB36" s="34"/>
+      <c r="BB36" s="35"/>
     </row>
     <row r="37" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="34"/>
-      <c r="E37" s="33"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="34"/>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="36"/>
-      <c r="M37" s="36"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="33"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="36"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="34"/>
       <c r="P37" s="28"/>
       <c r="Q37" s="28"/>
       <c r="R37" s="28"/>
-      <c r="S37" s="34"/>
-      <c r="T37" s="33"/>
+      <c r="S37" s="35"/>
+      <c r="T37" s="34"/>
       <c r="U37" s="28"/>
       <c r="V37" s="28"/>
       <c r="W37" s="28"/>
-      <c r="X37" s="34"/>
-      <c r="Y37" s="33"/>
+      <c r="X37" s="35"/>
+      <c r="Y37" s="34"/>
       <c r="Z37" s="28"/>
       <c r="AA37" s="28"/>
       <c r="AB37" s="28"/>
-      <c r="AC37" s="34"/>
-      <c r="AD37" s="33"/>
+      <c r="AC37" s="35"/>
+      <c r="AD37" s="34"/>
       <c r="AE37" s="28"/>
       <c r="AF37" s="28"/>
       <c r="AG37" s="28"/>
-      <c r="AH37" s="34"/>
-      <c r="AI37" s="58"/>
+      <c r="AH37" s="35"/>
+      <c r="AI37" s="59"/>
       <c r="AJ37" s="28"/>
       <c r="AK37" s="28"/>
       <c r="AL37" s="28"/>
-      <c r="AM37" s="34"/>
-      <c r="AN37" s="33"/>
+      <c r="AM37" s="35"/>
+      <c r="AN37" s="34"/>
       <c r="AO37" s="28"/>
       <c r="AP37" s="28"/>
       <c r="AQ37" s="28"/>
-      <c r="AR37" s="34"/>
-      <c r="AS37" s="33"/>
+      <c r="AR37" s="35"/>
+      <c r="AS37" s="34"/>
       <c r="AT37" s="28"/>
       <c r="AU37" s="28"/>
       <c r="AV37" s="28"/>
-      <c r="AW37" s="34"/>
-      <c r="AX37" s="33"/>
+      <c r="AW37" s="35"/>
+      <c r="AX37" s="34"/>
       <c r="AY37" s="28"/>
       <c r="AZ37" s="28"/>
       <c r="BA37" s="28"/>
-      <c r="BB37" s="34"/>
+      <c r="BB37" s="35"/>
     </row>
     <row r="38" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C38" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-      <c r="M38" s="36"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="33"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="37"/>
+      <c r="L38" s="37"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="34"/>
       <c r="P38" s="28"/>
       <c r="Q38" s="28"/>
       <c r="R38" s="28"/>
-      <c r="S38" s="34"/>
-      <c r="T38" s="33"/>
+      <c r="S38" s="35"/>
+      <c r="T38" s="34"/>
       <c r="U38" s="28"/>
       <c r="V38" s="28"/>
       <c r="W38" s="28"/>
-      <c r="X38" s="34"/>
-      <c r="Y38" s="33"/>
+      <c r="X38" s="35"/>
+      <c r="Y38" s="34"/>
       <c r="Z38" s="28"/>
       <c r="AA38" s="28"/>
       <c r="AB38" s="28"/>
-      <c r="AC38" s="34"/>
-      <c r="AD38" s="33"/>
+      <c r="AC38" s="35"/>
+      <c r="AD38" s="34"/>
       <c r="AE38" s="28"/>
       <c r="AF38" s="28"/>
       <c r="AG38" s="28"/>
-      <c r="AH38" s="34"/>
-      <c r="AI38" s="33"/>
+      <c r="AH38" s="35"/>
+      <c r="AI38" s="34"/>
       <c r="AJ38" s="28"/>
       <c r="AK38" s="28"/>
       <c r="AL38" s="28"/>
-      <c r="AM38" s="34"/>
-      <c r="AN38" s="33"/>
+      <c r="AM38" s="35"/>
+      <c r="AN38" s="34"/>
       <c r="AO38" s="28"/>
       <c r="AP38" s="28"/>
       <c r="AQ38" s="28"/>
-      <c r="AR38" s="34"/>
-      <c r="AS38" s="33"/>
+      <c r="AR38" s="35"/>
+      <c r="AS38" s="34"/>
       <c r="AT38" s="28"/>
       <c r="AU38" s="28"/>
       <c r="AV38" s="28"/>
-      <c r="AW38" s="34"/>
-      <c r="AX38" s="58"/>
+      <c r="AW38" s="35"/>
+      <c r="AX38" s="59"/>
       <c r="AY38" s="28"/>
       <c r="AZ38" s="28"/>
       <c r="BA38" s="28"/>
-      <c r="BB38" s="34"/>
+      <c r="BB38" s="35"/>
     </row>
     <row r="39" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="33"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="34"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="33"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="34"/>
       <c r="P39" s="28"/>
       <c r="Q39" s="28"/>
       <c r="R39" s="28"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="33"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="34"/>
       <c r="U39" s="28"/>
       <c r="V39" s="28"/>
       <c r="W39" s="28"/>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="33"/>
+      <c r="X39" s="35"/>
+      <c r="Y39" s="34"/>
       <c r="Z39" s="28"/>
       <c r="AA39" s="28"/>
       <c r="AB39" s="28"/>
-      <c r="AC39" s="34"/>
-      <c r="AD39" s="33"/>
+      <c r="AC39" s="35"/>
+      <c r="AD39" s="34"/>
       <c r="AE39" s="28"/>
       <c r="AF39" s="28"/>
       <c r="AG39" s="28"/>
-      <c r="AH39" s="34"/>
-      <c r="AI39" s="33"/>
+      <c r="AH39" s="35"/>
+      <c r="AI39" s="34"/>
       <c r="AJ39" s="28"/>
       <c r="AK39" s="28"/>
       <c r="AL39" s="28"/>
-      <c r="AM39" s="34"/>
-      <c r="AN39" s="33"/>
+      <c r="AM39" s="35"/>
+      <c r="AN39" s="34"/>
       <c r="AO39" s="28"/>
       <c r="AP39" s="28"/>
       <c r="AQ39" s="28"/>
-      <c r="AR39" s="34"/>
-      <c r="AS39" s="33"/>
+      <c r="AR39" s="35"/>
+      <c r="AS39" s="34"/>
       <c r="AT39" s="28"/>
       <c r="AU39" s="28"/>
       <c r="AV39" s="28"/>
-      <c r="AW39" s="34"/>
-      <c r="AX39" s="33"/>
+      <c r="AW39" s="35"/>
+      <c r="AX39" s="34"/>
       <c r="AY39" s="28"/>
       <c r="AZ39" s="28"/>
       <c r="BA39" s="28"/>
-      <c r="BB39" s="59"/>
+      <c r="BB39" s="60"/>
     </row>
     <row r="40" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C40" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
       <c r="F40" s="28"/>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="35"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
-      <c r="N40" s="37"/>
-      <c r="O40" s="33"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="37"/>
+      <c r="L40" s="37"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="34"/>
       <c r="P40" s="28"/>
       <c r="Q40" s="28"/>
       <c r="R40" s="28"/>
-      <c r="S40" s="34"/>
-      <c r="T40" s="33"/>
+      <c r="S40" s="35"/>
+      <c r="T40" s="34"/>
       <c r="U40" s="28"/>
       <c r="V40" s="28"/>
       <c r="W40" s="28"/>
-      <c r="X40" s="34"/>
-      <c r="Y40" s="33"/>
+      <c r="X40" s="35"/>
+      <c r="Y40" s="34"/>
       <c r="Z40" s="28"/>
       <c r="AA40" s="28"/>
       <c r="AB40" s="28"/>
-      <c r="AC40" s="34"/>
-      <c r="AD40" s="33"/>
+      <c r="AC40" s="35"/>
+      <c r="AD40" s="34"/>
       <c r="AE40" s="28"/>
       <c r="AF40" s="28"/>
       <c r="AG40" s="28"/>
-      <c r="AH40" s="34"/>
-      <c r="AI40" s="33"/>
+      <c r="AH40" s="35"/>
+      <c r="AI40" s="34"/>
       <c r="AJ40" s="28"/>
       <c r="AK40" s="28"/>
       <c r="AL40" s="28"/>
-      <c r="AM40" s="34"/>
-      <c r="AN40" s="33"/>
+      <c r="AM40" s="35"/>
+      <c r="AN40" s="34"/>
       <c r="AO40" s="28"/>
       <c r="AP40" s="28"/>
       <c r="AQ40" s="28"/>
-      <c r="AR40" s="34"/>
-      <c r="AS40" s="33"/>
+      <c r="AR40" s="35"/>
+      <c r="AS40" s="34"/>
       <c r="AT40" s="28"/>
       <c r="AU40" s="28"/>
       <c r="AV40" s="28"/>
-      <c r="AW40" s="34"/>
-      <c r="AX40" s="33"/>
+      <c r="AW40" s="35"/>
+      <c r="AX40" s="34"/>
       <c r="AY40" s="28"/>
       <c r="AZ40" s="28"/>
       <c r="BA40" s="28"/>
-      <c r="BB40" s="59"/>
+      <c r="BB40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0"/>
@@ -4521,13 +4433,13 @@
       </c>
     </row>
     <row r="49" s="12" customFormat="true" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="39"/>
+      <c r="A49" s="40"/>
       <c r="C49" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="50" s="12" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="39"/>
+      <c r="A50" s="40"/>
       <c r="C50" s="68" t="s">
         <v>67</v>
       </c>
@@ -4578,7 +4490,7 @@
   </sheetPr>
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -4651,7 +4563,7 @@
       <c r="F5" s="76"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="73"/>
       <c r="C6" s="74"/>
       <c r="D6" s="75"/>
@@ -4772,7 +4684,7 @@
   </sheetPr>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
@@ -4802,61 +4714,61 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="39"/>
+      <c r="A2" s="40"/>
       <c r="B2" s="73"/>
       <c r="C2" s="85"/>
       <c r="D2" s="73"/>
     </row>
     <row r="3" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="73"/>
       <c r="C3" s="85"/>
       <c r="D3" s="73"/>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="73"/>
       <c r="C4" s="85"/>
       <c r="D4" s="73"/>
     </row>
     <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="73"/>
       <c r="C5" s="85"/>
       <c r="D5" s="73"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="73"/>
       <c r="C6" s="85"/>
       <c r="D6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="73"/>
       <c r="C7" s="85"/>
       <c r="D7" s="73"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="73"/>
       <c r="C8" s="85"/>
       <c r="D8" s="73"/>
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="39"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="73"/>
       <c r="C9" s="85"/>
       <c r="D9" s="73"/>
     </row>
     <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="73"/>
       <c r="C10" s="85"/>
       <c r="D10" s="73"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="73"/>
       <c r="C11" s="85"/>
       <c r="D11" s="73"/>
@@ -4883,55 +4795,55 @@
       <c r="A15" s="86"/>
       <c r="B15" s="73"/>
       <c r="C15" s="85"/>
-      <c r="D15" s="39"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="86"/>
       <c r="B16" s="73"/>
       <c r="C16" s="85"/>
-      <c r="D16" s="39"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="86"/>
       <c r="B17" s="73"/>
       <c r="C17" s="85"/>
-      <c r="D17" s="39"/>
+      <c r="D17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="86"/>
       <c r="B18" s="73"/>
       <c r="C18" s="85"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="86"/>
       <c r="B19" s="73"/>
       <c r="C19" s="85"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="86"/>
       <c r="B20" s="73"/>
       <c r="C20" s="85"/>
-      <c r="D20" s="39"/>
+      <c r="D20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="86"/>
       <c r="B21" s="73"/>
       <c r="C21" s="85"/>
-      <c r="D21" s="39"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="86"/>
       <c r="B22" s="73"/>
       <c r="C22" s="85"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="86"/>
       <c r="B23" s="73"/>
       <c r="C23" s="85"/>
-      <c r="D23" s="39"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="86"/>
@@ -5100,7 +5012,7 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -5252,7 +5164,7 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="56" zoomScaleNormal="56" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -5260,7 +5172,7 @@
       <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="98" width="10"/>

</xml_diff>